<commit_message>
UPDATED data, affectedpop and cost1
</commit_message>
<xml_diff>
--- a/DataSets/Calumpit community data.xlsx
+++ b/DataSets/Calumpit community data.xlsx
@@ -416,7 +416,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -466,7 +466,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -486,7 +486,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -506,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -566,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -606,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>6</v>
       </c>
       <c r="F10">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>115</v>
       </c>
       <c r="F11">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
         <v>57</v>
       </c>
       <c r="F12">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>601</v>
       </c>
       <c r="F14">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -746,7 +746,7 @@
         <v>56</v>
       </c>
       <c r="F16">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>6</v>
       </c>
       <c r="F17">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -786,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -806,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
         <v>92</v>
       </c>
       <c r="F20">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -886,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -926,7 +926,7 @@
         <v>17</v>
       </c>
       <c r="F25">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -946,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -966,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
         <v>65</v>
       </c>
       <c r="F28">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1026,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>1000</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
refactor xDeg, yDeg to Latitude, Longitude; Fixed headers in EntityMan
</commit_message>
<xml_diff>
--- a/DataSets/Calumpit community data.xlsx
+++ b/DataSets/Calumpit community data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL\BRYAN\bulsu\Thesis 1\ShelterAlloc_Thesis\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070711E2-3839-4AB7-800C-584A6AE43F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9254A6-B666-4D3B-B804-8C5C28FC2925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>Population</t>
-  </si>
-  <si>
-    <t>xDegrees</t>
-  </si>
-  <si>
-    <t>yDegrees</t>
   </si>
   <si>
     <t>Name</t>
@@ -139,6 +133,12 @@
   </si>
   <si>
     <t>Sucol</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -429,22 +429,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>14.8956</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>14.914300000000001</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>14.894</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>14.9076</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>14.9125</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>14.884499999999999</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>14.9054</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>14.912800000000001</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>14.9153</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>14.921799999999999</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>14.901400000000001</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>14.889900000000001</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>14.8919</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>14.8748</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>14.9078</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>14.883100000000001</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>14.8994</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>14.876099999999999</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>14.8881</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>14.915699999999999</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>14.9023</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>14.883800000000001</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>14.897600000000001</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>14.917</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>14.898199999999999</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>14.9047</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>14.919600000000001</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>14.894</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>14.9138</v>

</xml_diff>